<commit_message>
updated in-class instructions and starter sheet
</commit_message>
<xml_diff>
--- a/docs/unit1/1_analyzing_managing_data/(Starter-Workbook)-Class-Analyzing-&-Managing-Data.xlsx
+++ b/docs/unit1/1_analyzing_managing_data/(Starter-Workbook)-Class-Analyzing-&-Managing-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bw383\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005BDEBF-2E3D-46BA-BA38-8C1C7CA52F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67D6A99-DCC5-5E45-8FC4-8FFF5E576885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24680" yWindow="1120" windowWidth="35400" windowHeight="24360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company Inventory" sheetId="1" r:id="rId1"/>
@@ -121,6 +121,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -128,6 +129,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -135,39 +137,46 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -175,6 +184,7 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -186,7 +196,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,32 +211,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8BC34A"/>
-        <bgColor rgb="FF8BC34A"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
-        <bgColor rgb="FFD9EAD3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF666666"/>
         <bgColor rgb="FF666666"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEBEFF1"/>
-        <bgColor rgb="FFEBEFF1"/>
       </patternFill>
     </fill>
     <fill>
@@ -241,6 +233,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF78909C"/>
+        <bgColor rgb="FF78909C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor rgb="FF8BC34A"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -254,110 +258,7 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
       <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -419,32 +320,47 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -452,10 +368,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -470,7 +386,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -482,13 +398,28 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -500,26 +431,94 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -527,54 +526,31 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -587,8 +563,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="43">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -598,7 +574,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -606,115 +581,84 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,42 +692,6 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -848,12 +756,48 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1124,23 +1068,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="A2:D20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A23:D23" headerRowCount="0" headerRowDxfId="6" totalsRowDxfId="4" tableBorderDxfId="5">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Day"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Temp (F)"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Temp (C)"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Temp (K)"/>
-  </tableColumns>
-  <tableStyleInfo name="Temperature Conversions-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A23:D23" headerRowCount="0" headerRowDxfId="2" totalsRowDxfId="1" tableBorderDxfId="6">
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Column2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Column3" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Column2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Column3" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Column4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Temperature Conversions-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
@@ -1149,17 +1081,6 @@
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
     </ext>
   </extLst>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_5" displayName="Table_5" ref="B24:D28" headerRowCount="0">
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Column3"/>
-  </tableColumns>
-  <tableStyleInfo name="Temperature Conversions-style 3" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1364,121 +1285,121 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-    </row>
-    <row r="2" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+    </row>
+    <row r="2" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="39" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="34">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A3" s="40">
         <v>45547</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="42">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="36">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A4" s="40">
         <v>45548</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="42">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="34">
+    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A5" s="40">
         <v>45549</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="42">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="36">
+    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A6" s="40">
         <v>45550</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="42">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="34">
+    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A7" s="40">
         <v>45551</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="42">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="36">
+    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A8" s="40">
         <v>45552</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="42">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="34">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="40">
         <v>45553</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="42">
         <v>6</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="36">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="40">
         <v>45554</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="41" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="42">
@@ -1486,23 +1407,23 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="34">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="40">
         <v>45555</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="42">
         <v>5</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="36">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="40">
         <v>45556</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="42">
@@ -1510,23 +1431,23 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="34">
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="40">
         <v>45557</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13" s="42">
         <v>21</v>
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="36">
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="40">
         <v>45558</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="42">
@@ -1534,23 +1455,21 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="38" t="s">
+    <row r="16" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
-    </row>
-    <row r="18" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="12.75" x14ac:dyDescent="0.2"/>
+      <c r="C16" s="36"/>
+    </row>
+    <row r="19" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="20" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="21" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="22" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="23" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="24" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1567,15 +1486,15 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="5" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="5" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1584,7 +1503,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1601,435 +1520,435 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>1001</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>76</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>76</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>46</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>76</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
         <v>1002</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>70</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>89</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>100</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>63</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>1003</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>57</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>81</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>73</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>67</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
         <v>1004</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>91</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>100</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>41</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>30</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
         <v>1005</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>88</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>100</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>62</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>75</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
         <v>1006</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>80</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>68</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>55</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>78</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
         <v>1007</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>84</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>44</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>50</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
         <v>1008</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>95</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>24</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>61</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
         <v>1009</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>53</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>98</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>66</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
         <v>1010</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>58</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>54</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>35</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4">
         <v>1011</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>58</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>63</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>34</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4">
         <v>1012</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>63</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>59</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>80</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
         <v>1013</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>86</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>57</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>56</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4">
         <v>1014</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>97</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>51</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>47</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4">
         <v>1015</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>64</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>45</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>22</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4">
         <v>1016</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>90</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>59</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>32</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>1017</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>76</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>100</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>0</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4">
         <v>1018</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>68</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>15</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>28</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4">
         <v>1019</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>76</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>47</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <v>23</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4">
         <v>1020</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>83</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>87</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>89</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4">
         <v>1021</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>56</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>90</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <v>58</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4">
         <v>1022</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>100</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>84</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <v>10</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4">
         <v>1023</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>98</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>97</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <v>95</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4">
         <v>1024</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <v>98</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>17</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <v>71</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <v>89</v>
       </c>
     </row>
@@ -2045,202 +1964,202 @@
   </sheetPr>
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="10"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="14">
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A3" s="24">
         <v>45547</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="25">
         <v>32</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="14">
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A4" s="24">
         <v>45548</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="25">
         <v>88</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="14">
+      <c r="C4" s="26"/>
+      <c r="D4" s="27"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A5" s="24">
         <v>45549</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="25">
         <v>21</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="14">
+      <c r="C5" s="26"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A6" s="24">
         <v>45550</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="25">
         <v>41</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="14">
+      <c r="C6" s="26"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A7" s="24">
         <v>45551</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="25">
         <v>65</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="14">
+      <c r="C7" s="26"/>
+      <c r="D7" s="27"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A8" s="24">
         <v>45552</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="25">
         <v>78</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="14">
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A9" s="24">
         <v>45553</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="25">
         <v>27</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="14">
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A10" s="24">
         <v>45554</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="25">
         <v>25</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="14">
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A11" s="24">
         <v>45555</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="25">
         <v>25</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="14">
+    <row r="12" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A12" s="24">
         <v>45556</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="25">
         <v>98</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="14">
+    <row r="13" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A13" s="24">
         <v>45557</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="25">
         <v>16</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="17"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -2248,141 +2167,141 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="14">
+    <row r="14" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A14" s="24">
         <v>45558</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="25">
         <v>66</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="17"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="14">
+    <row r="15" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A15" s="24">
         <v>45559</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="25">
         <v>77</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="17"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="14">
+    <row r="16" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="A16" s="24">
         <v>45560</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="25">
         <v>89</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="17"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="14">
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
+    </row>
+    <row r="17" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A17" s="24">
         <v>45561</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="25">
         <v>41</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="14">
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A18" s="24">
         <v>45562</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="25">
         <v>42</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="17"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="14">
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
+    </row>
+    <row r="19" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A19" s="24">
         <v>45563</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="25">
         <v>75</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="17"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="22">
+      <c r="C19" s="26"/>
+      <c r="D19" s="27"/>
+    </row>
+    <row r="20" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A20" s="28">
         <v>45564</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="29">
         <v>8</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="31"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="47"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="48" t="s">
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="49" t="s">
+      <c r="D23" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="50" t="s">
+    <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A24" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="51"/>
-    </row>
-    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="50" t="s">
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="33"/>
+    </row>
+    <row r="25" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A25" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="51"/>
-    </row>
-    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="50" t="s">
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="33"/>
+    </row>
+    <row r="26" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A26" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="51"/>
-    </row>
-    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="50" t="s">
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="33"/>
+    </row>
+    <row r="27" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A27" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="51"/>
-    </row>
-    <row r="28" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="52" t="s">
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="33"/>
+    </row>
+    <row r="28" spans="1:5" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="54"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2392,10 +2311,8 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="3">
+  <tableParts count="1">
     <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>